<commit_message>
Assignment 1 - Test Case for Creating Account on BDJobs
</commit_message>
<xml_diff>
--- a/Test Case 1 - BdJobs/Create Account Test Case for BdJobs.xlsx
+++ b/Test Case 1 - BdJobs/Create Account Test Case for BdJobs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash\Desktop\Test-Case-Writing\Test Case 1 - BdJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ACFC6A-1323-44B5-960C-5AFB77C2699E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D8C8B-6344-48A2-A5FE-0E63FF66C690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D41CCF6-EEAA-4CAF-AB7E-877FBCAA033C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="205">
   <si>
     <t>TEST TITLE</t>
   </si>
@@ -483,6 +483,177 @@
   </si>
   <si>
     <t>An error appeared that the "Name maximum 100 characters."</t>
+  </si>
+  <si>
+    <t>Providing special characters at the 'Phone Number' field</t>
+  </si>
+  <si>
+    <t>@@##</t>
+  </si>
+  <si>
+    <t>An error should appear that "Invalid Phone Number"</t>
+  </si>
+  <si>
+    <t>0173@qw</t>
+  </si>
+  <si>
+    <t>Providing combination of digits, alpha, and special characters at the 'Phone Number' field</t>
+  </si>
+  <si>
+    <t>The "Phone Number" field should not accept alpha characters.</t>
+  </si>
+  <si>
+    <t>The "Phone Number" field should not accept special characters.</t>
+  </si>
+  <si>
+    <t>The "Phone Number" field did not accept alpha or special characters.</t>
+  </si>
+  <si>
+    <t>Only 0173 was accepeted as input</t>
+  </si>
+  <si>
+    <t>Providing other country numbers at the 'Phone Number' field</t>
+  </si>
+  <si>
+    <t>9194762803</t>
+  </si>
+  <si>
+    <t>An error should appear that "only Bangladeshi number is accepted"</t>
+  </si>
+  <si>
+    <t>An error appeared that "Invalid mobile number"</t>
+  </si>
+  <si>
+    <t>USA Number</t>
+  </si>
+  <si>
+    <t>Check if the field accepts whitespace in between numbers</t>
+  </si>
+  <si>
+    <t>017 781770073</t>
+  </si>
+  <si>
+    <t>The "Phone Number" field should not accept blackspace</t>
+  </si>
+  <si>
+    <t>The "Phone Number" field did not accept space</t>
+  </si>
+  <si>
+    <t>Providing invalid operator code at the 'Phone Number' field</t>
+  </si>
+  <si>
+    <t>01281770073</t>
+  </si>
+  <si>
+    <t>01281770073          01181770073</t>
+  </si>
+  <si>
+    <t>Valid Bangladeshi operators are 019,018,017,015,016,013,014</t>
+  </si>
+  <si>
+    <t>Testing the Password Filed</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>1.1,1.2,1.3,1.5,1.4,1.6,1.9</t>
+  </si>
+  <si>
+    <t>4.1 0</t>
+  </si>
+  <si>
+    <t>Keeping the "Password" &amp; "Confirm Password" field empty and fill the other fields with valid data</t>
+  </si>
+  <si>
+    <t>An error should appear that the password is required.</t>
+  </si>
+  <si>
+    <t>An error appeared that the "Please enter Password."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Providing a valid password and invalid confirm password </t>
+  </si>
+  <si>
+    <t>123@@akash         123@@batash</t>
+  </si>
+  <si>
+    <t>An error should appear that the confirm password is not matched.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Providing seven character password and confirm password &amp; fill the other fields with valid data. </t>
+  </si>
+  <si>
+    <t>An error appeared that the "These Passwords don't match."</t>
+  </si>
+  <si>
+    <t>123one7</t>
+  </si>
+  <si>
+    <t>An error appeared that the "Password minimum 8 characters."</t>
+  </si>
+  <si>
+    <t>Providing more than 12 character password and confirm password</t>
+  </si>
+  <si>
+    <t>one@two#3$four</t>
+  </si>
+  <si>
+    <t>An error should appear that "The password should be at least 8 characters"</t>
+  </si>
+  <si>
+    <t>An error should appear that "The password can't exceed 12 characters."</t>
+  </si>
+  <si>
+    <t>More than 12 characters can't be typed.</t>
+  </si>
+  <si>
+    <t>Verify if the password is only numbers</t>
+  </si>
+  <si>
+    <t>An error should appear that "At least 1 letter, 1 unique character should be included in the password."</t>
+  </si>
+  <si>
+    <t>The registration was completed with a week password</t>
+  </si>
+  <si>
+    <t>Verify if the password is only alpha characters</t>
+  </si>
+  <si>
+    <t>onetwothree</t>
+  </si>
+  <si>
+    <t>Verify if the password is only special characters</t>
+  </si>
+  <si>
+    <t>@#$#@#@#</t>
+  </si>
+  <si>
+    <t>Verify if the password contains name of the user</t>
+  </si>
+  <si>
+    <t>AsmaulAkash</t>
+  </si>
+  <si>
+    <t>An error should appear that "Name can't be used as password"</t>
+  </si>
+  <si>
+    <t>The registration was completed with same name &amp; password</t>
+  </si>
+  <si>
+    <t>Providing only whitespaces as password</t>
+  </si>
+  <si>
+    <t>An error should appear that "Space can't be used as password."</t>
+  </si>
+  <si>
+    <t>An error appeared that the "Please use only letters (a-z), numbers (0-9) and punctuations."</t>
+  </si>
+  <si>
+    <t>Providing only punctuations as password</t>
+  </si>
+  <si>
+    <t>….......</t>
   </si>
 </sst>
 </file>
@@ -816,7 +987,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -923,15 +1094,21 @@
     <xf numFmtId="164" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -978,9 +1155,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1302,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C43487-EE7C-4092-98D5-12C25A679693}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J118" sqref="J118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,10 +1567,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="38"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="22" t="s">
         <v>5</v>
       </c>
@@ -1408,10 +1582,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
@@ -1464,13 +1638,13 @@
       <c r="D21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="47" t="s">
+      <c r="G21" s="49" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="14"/>
@@ -1485,9 +1659,9 @@
       <c r="D22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="51"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="48"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,9 +1674,9 @@
       <c r="D23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="48"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1515,9 +1689,9 @@
       <c r="D24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="48"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1530,25 +1704,25 @@
       <c r="D25" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="48"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="50"/>
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="45" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="41" t="s">
+      <c r="E26" s="53"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="43" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1556,14 +1730,14 @@
       <c r="B27" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="42"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="44"/>
     </row>
     <row r="28" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="24">
@@ -1572,12 +1746,12 @@
       <c r="C28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="48"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,10 +1761,10 @@
       <c r="C29" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1603,9 +1777,9 @@
       <c r="D30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="49"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="14"/>
     </row>
     <row r="33" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1644,10 +1818,10 @@
     </row>
     <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="38"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="22" t="s">
         <v>5</v>
       </c>
@@ -1659,10 +1833,10 @@
       </c>
     </row>
     <row r="37" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="40"/>
+      <c r="D37" s="41"/>
       <c r="E37" s="8" t="s">
         <v>22</v>
       </c>
@@ -2033,10 +2207,10 @@
     </row>
     <row r="59" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C60" s="38" t="s">
+      <c r="C60" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="38"/>
+      <c r="D60" s="42"/>
       <c r="E60" s="22" t="s">
         <v>5</v>
       </c>
@@ -2048,10 +2222,10 @@
       </c>
     </row>
     <row r="61" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="39" t="s">
+      <c r="C61" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="40"/>
+      <c r="D61" s="41"/>
       <c r="E61" s="8" t="s">
         <v>22</v>
       </c>
@@ -2283,125 +2457,137 @@
       </c>
       <c r="H72" s="35"/>
     </row>
-    <row r="77" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="24"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="14"/>
-    </row>
-    <row r="81" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C81" s="22" t="s">
+    <row r="80" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C80" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D81" s="23" t="s">
+      <c r="D80" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E81" s="22" t="s">
+      <c r="E80" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F81" s="23" t="s">
+      <c r="F80" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G81" s="23" t="s">
+      <c r="G80" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="7" t="s">
+    <row r="81" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F81" s="6">
         <v>1</v>
       </c>
-      <c r="G82" s="6" t="s">
+      <c r="G81" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C84" s="38" t="s">
+    <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C83" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D84" s="38"/>
-      <c r="E84" s="22" t="s">
+      <c r="D83" s="42"/>
+      <c r="E83" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F84" s="22" t="s">
+      <c r="F83" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G84" s="23" t="s">
+      <c r="G83" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C85" s="39" t="s">
+    <row r="84" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="D85" s="40"/>
-      <c r="E85" s="8" t="s">
+      <c r="D84" s="41"/>
+      <c r="E84" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F84" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="G84" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="16" t="s">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C86" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D87" s="18" t="s">
+      <c r="D86" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E86" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F87" s="20" t="s">
+      <c r="F86" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G87" s="21" t="s">
+      <c r="G86" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H87" s="15" t="s">
+      <c r="H86" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="24">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D87" s="13"/>
+      <c r="E87" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G87" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H87" s="14"/>
+    </row>
+    <row r="88" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="24">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D88" s="13"/>
+        <v>128</v>
+      </c>
+      <c r="D88" s="39" t="s">
+        <v>132</v>
+      </c>
       <c r="E88" s="26" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F88" s="27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G88" s="28" t="s">
         <v>27</v>
@@ -2410,13 +2596,13 @@
     </row>
     <row r="89" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="24">
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D89" s="57" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>131</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>135</v>
@@ -2431,19 +2617,19 @@
     </row>
     <row r="90" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="24">
-        <v>3.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D90" s="56" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="D90" s="38" t="s">
+        <v>134</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F90" s="27" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G90" s="28" t="s">
         <v>27</v>
@@ -2452,76 +2638,466 @@
     </row>
     <row r="91" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="24">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="56" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>138</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F91" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="G91" s="28" t="s">
-        <v>27</v>
+        <v>140</v>
+      </c>
+      <c r="G91" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="H91" s="14"/>
     </row>
     <row r="92" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="24">
-        <v>3.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="D92" s="56" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="D92" s="38" t="s">
+        <v>142</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="F92" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="G92" s="30" t="s">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="G92" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="H92" s="14"/>
     </row>
     <row r="93" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="24">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D93" s="56" t="s">
-        <v>142</v>
+        <v>148</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>149</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="G93" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G93" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H93" s="14"/>
+    </row>
+    <row r="94" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="24">
+        <v>4.8</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D94" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E94" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F94" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G94" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="24">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D95" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E95" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F95" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="G95" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H95" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="F96" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G96" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H96" s="14"/>
+    </row>
+    <row r="97" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="24">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D97" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="E97" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F97" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G97" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H97" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G102" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F103" s="6">
+        <v>1</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C105" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="42"/>
+      <c r="E105" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D106" s="41"/>
+      <c r="E106" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E108" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G108" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H108" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D109" s="13"/>
+      <c r="E109" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F109" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="G109" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H109" s="14"/>
+    </row>
+    <row r="110" spans="2:8" s="10" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="24">
+        <v>5.2</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D110" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F110" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="G110" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H110" s="14"/>
+    </row>
+    <row r="111" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="24">
+        <v>5.3</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D111" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F111" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="G111" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H111" s="14"/>
+    </row>
+    <row r="112" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="24">
+        <v>5.4</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D112" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="E112" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="F112" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G112" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H112" s="14"/>
+    </row>
+    <row r="113" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="24">
+        <v>5.5</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D113" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F113" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G113" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H93" s="14"/>
+      <c r="H113" s="14"/>
+    </row>
+    <row r="114" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="24">
+        <v>5.6</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D114" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="E114" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F114" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G114" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H114" s="14"/>
+    </row>
+    <row r="115" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="24">
+        <v>5.6</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D115" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F115" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G115" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H115" s="14"/>
+    </row>
+    <row r="116" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="24">
+        <v>5.7</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D116" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F116" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G116" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H116" s="14"/>
+    </row>
+    <row r="117" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="24">
+        <v>5.8</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D117" s="37"/>
+      <c r="E117" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="F117" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="G117" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H117" s="14"/>
+    </row>
+    <row r="118" spans="2:8" s="10" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="24">
+        <v>5.8</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D118" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="E118" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F118" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G118" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H118" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C37:D37"/>
+  <mergeCells count="16">
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="C26:C27"/>
@@ -2529,6 +3105,11 @@
     <mergeCell ref="G21:G30"/>
     <mergeCell ref="E21:E30"/>
     <mergeCell ref="F21:F30"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C37:D37"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A9">
     <cfRule type="colorScale" priority="5">
@@ -2543,13 +3124,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15 D34 D82 D58" xr:uid="{940F4261-569D-4DC3-AD05-736585928CB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15 D34 D81 D58 D103" xr:uid="{940F4261-569D-4DC3-AD05-736585928CB6}">
       <formula1>"HIGH, MEDIUM, LOW"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15 G34 G82 G58" xr:uid="{7AC68441-3FCF-4CD5-B822-EB9A4062ABAD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15 G34 G81 G58 G103" xr:uid="{7AC68441-3FCF-4CD5-B822-EB9A4062ABAD}">
       <formula1>"DUPLICATE, ON GOING, TEST DONE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21 G77 G88:G93 G64:G72 G40:G53" xr:uid="{073FB9ED-BFBC-4F46-A2B5-AC54E05E9F87}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21 G40:G53 G64:G72 G87:G97 G109:G118" xr:uid="{073FB9ED-BFBC-4F46-A2B5-AC54E05E9F87}">
       <formula1>"PASS, FAIL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Assignment 1 - Create Accunt Test Case
</commit_message>
<xml_diff>
--- a/Test Case 1 - BdJobs/Create Account Test Case for BdJobs.xlsx
+++ b/Test Case 1 - BdJobs/Create Account Test Case for BdJobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash\Desktop\Test-Case-Writing\Test Case 1 - BdJobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D8C8B-6344-48A2-A5FE-0E63FF66C690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF7E269-8320-47B4-B06B-627F033BC69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D41CCF6-EEAA-4CAF-AB7E-877FBCAA033C}"/>
   </bookViews>
@@ -1100,15 +1100,18 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1153,9 +1156,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C43487-EE7C-4092-98D5-12C25A679693}">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="42"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="22" t="s">
         <v>5</v>
       </c>
@@ -1582,10 +1582,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
@@ -1638,13 +1638,13 @@
       <c r="D21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="55" t="s">
+      <c r="F21" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="50" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="14"/>
@@ -1659,9 +1659,9 @@
       <c r="D22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="50"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,9 +1674,9 @@
       <c r="D23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="53"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="50"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,9 +1689,9 @@
       <c r="D24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="53"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="50"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1704,25 +1704,25 @@
       <c r="D25" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="53"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="50"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="46" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="43" t="s">
+      <c r="E26" s="54"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="44" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1730,14 +1730,14 @@
       <c r="B27" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="46"/>
+      <c r="C27" s="47"/>
       <c r="D27" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="53"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="44"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="24">
@@ -1746,12 +1746,12 @@
       <c r="C28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="50"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1761,10 +1761,10 @@
       <c r="C29" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="50"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1777,9 +1777,9 @@
       <c r="D30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="54"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="51"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="52"/>
       <c r="H30" s="14"/>
     </row>
     <row r="33" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1818,10 +1818,10 @@
     </row>
     <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="42"/>
+      <c r="D36" s="41"/>
       <c r="E36" s="22" t="s">
         <v>5</v>
       </c>
@@ -1833,10 +1833,10 @@
       </c>
     </row>
     <row r="37" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="41"/>
+      <c r="D37" s="43"/>
       <c r="E37" s="8" t="s">
         <v>22</v>
       </c>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="59" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C60" s="42" t="s">
+      <c r="C60" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="42"/>
+      <c r="D60" s="41"/>
       <c r="E60" s="22" t="s">
         <v>5</v>
       </c>
@@ -2222,10 +2222,10 @@
       </c>
     </row>
     <row r="61" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="40" t="s">
+      <c r="C61" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="41"/>
+      <c r="D61" s="43"/>
       <c r="E61" s="8" t="s">
         <v>22</v>
       </c>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C83" s="42" t="s">
+      <c r="C83" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="42"/>
+      <c r="D83" s="41"/>
       <c r="E83" s="22" t="s">
         <v>5</v>
       </c>
@@ -2508,10 +2508,10 @@
       </c>
     </row>
     <row r="84" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C84" s="40" t="s">
+      <c r="C84" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D84" s="41"/>
+      <c r="D84" s="43"/>
       <c r="E84" s="8" t="s">
         <v>22</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="C97" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="D97" s="58" t="s">
+      <c r="D97" s="40" t="s">
         <v>168</v>
       </c>
       <c r="E97" s="26" t="s">
@@ -2825,10 +2825,10 @@
     </row>
     <row r="104" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="105" spans="2:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="42" t="s">
+      <c r="C105" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D105" s="42"/>
+      <c r="D105" s="41"/>
       <c r="E105" s="22" t="s">
         <v>5</v>
       </c>
@@ -2840,10 +2840,10 @@
       </c>
     </row>
     <row r="106" spans="2:8" s="5" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C106" s="40" t="s">
+      <c r="C106" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="D106" s="41"/>
+      <c r="D106" s="43"/>
       <c r="E106" s="8" t="s">
         <v>22</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="C113" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D113" s="58" t="s">
+      <c r="D113" s="40" t="s">
         <v>167</v>
       </c>
       <c r="E113" s="26" t="s">
@@ -2996,7 +2996,7 @@
       <c r="C114" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D114" s="58" t="s">
+      <c r="D114" s="40" t="s">
         <v>193</v>
       </c>
       <c r="E114" s="26" t="s">
@@ -3017,7 +3017,7 @@
       <c r="C115" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D115" s="58" t="s">
+      <c r="D115" s="40" t="s">
         <v>195</v>
       </c>
       <c r="E115" s="26" t="s">
@@ -3094,22 +3094,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="G21:G30"/>
     <mergeCell ref="E21:E30"/>
     <mergeCell ref="F21:F30"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A9">
     <cfRule type="colorScale" priority="5">

</xml_diff>